<commit_message>
Modified clock controlled IAV model based on IAV model
</commit_message>
<xml_diff>
--- a/detailed_model_1/data_to_fit.xlsx
+++ b/detailed_model_1/data_to_fit.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="95">
   <si>
     <t>CD45 cells (as % of all live cells)</t>
   </si>
@@ -231,35 +231,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>NK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ZT11</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>T</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>T_E</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>IL6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>CCL2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Neu</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -409,27 +389,63 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Lung CD8 Tcell (cell number)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lung CD8(cell number = CD45 at day 4 of ZT11 * % of cd45)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lung CD8_E (cell number = CD45 at day 4 of ZT11 * % of cd45)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lung CD8 Tcell (as % of all live cells) without T_E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lung CD8 Tcell (cell number) without T_E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZT23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>H</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Lung CD8 Tcell (cell number)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lung CD8(cell number = CD45 at day 4 of ZT11 * % of cd45)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lung CD8_E (cell number = CD45 at day 4 of ZT11 * % of cd45)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lung CD8 Tcell (as % of all live cells) without T_E</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lung CD8 Tcell (cell number) without T_E</t>
+    <t>ZT23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZT11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZT23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Neu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T_E</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -866,30 +882,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -923,15 +915,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -944,6 +927,39 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1246,33 +1262,33 @@
       <c r="E1" s="30"/>
       <c r="F1" s="30"/>
       <c r="G1" s="30"/>
-      <c r="L1" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
+      <c r="L1" s="69" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
     </row>
     <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="42" t="s">
+      <c r="C2" s="64"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="44"/>
-      <c r="L2" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="65"/>
+      <c r="L2" s="70" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
     </row>
     <row r="3" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1296,13 +1312,13 @@
       <c r="G3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
+      <c r="L3" s="69" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="69"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
@@ -1326,13 +1342,13 @@
       <c r="G4" s="9">
         <v>5</v>
       </c>
-      <c r="L4" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
+      <c r="L4" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="M4" s="70"/>
+      <c r="N4" s="70"/>
+      <c r="O4" s="70"/>
+      <c r="P4" s="70"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
@@ -1356,13 +1372,13 @@
       <c r="G5" s="9">
         <v>5</v>
       </c>
-      <c r="L5" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
+      <c r="L5" s="70" t="s">
+        <v>63</v>
+      </c>
+      <c r="M5" s="70"/>
+      <c r="N5" s="70"/>
+      <c r="O5" s="70"/>
+      <c r="P5" s="70"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
@@ -1411,7 +1427,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="48"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -1420,51 +1436,51 @@
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="L9" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="N9" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="O9" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="L9" s="51" t="s">
-        <v>3</v>
-      </c>
-      <c r="M9" s="52" t="s">
+      <c r="P9" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q9" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="R9" s="46" t="s">
         <v>72</v>
-      </c>
-      <c r="N9" s="53" t="s">
-        <v>73</v>
-      </c>
-      <c r="O9" s="53" t="s">
-        <v>74</v>
-      </c>
-      <c r="P9" s="53" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q9" s="53" t="s">
-        <v>76</v>
-      </c>
-      <c r="R9" s="54" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="45" t="s">
+      <c r="C10" s="67"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="46"/>
-      <c r="G10" s="47"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="68"/>
       <c r="L10" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="M10" s="37">
         <f>B12/B4*100</f>
@@ -1478,12 +1494,12 @@
         <f>B36*B12/100</f>
         <v>21.520399999999999</v>
       </c>
-      <c r="P10" s="57">
+      <c r="P10" s="49">
         <v>45.1</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="42" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1519,7 +1535,7 @@
         <f t="shared" ref="O11:O13" si="2">B37*B13/100</f>
         <v>60.931199999999997</v>
       </c>
-      <c r="P11" s="58">
+      <c r="P11" s="50">
         <v>56.2</v>
       </c>
     </row>
@@ -1560,7 +1576,7 @@
         <f t="shared" si="2"/>
         <v>68.062999999999988</v>
       </c>
-      <c r="P12" s="58">
+      <c r="P12" s="50">
         <v>61</v>
       </c>
     </row>
@@ -1601,7 +1617,7 @@
         <f t="shared" si="2"/>
         <v>99.531999999999982</v>
       </c>
-      <c r="P13" s="59">
+      <c r="P13" s="51">
         <v>70.3</v>
       </c>
     </row>
@@ -1628,7 +1644,7 @@
         <v>5</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="M14" s="37">
         <f>E12/E4*100</f>
@@ -1642,7 +1658,7 @@
         <f>E36*E12/100</f>
         <v>27.846</v>
       </c>
-      <c r="P14" s="57">
+      <c r="P14" s="49">
         <v>44.1</v>
       </c>
     </row>
@@ -1683,12 +1699,12 @@
         <f t="shared" ref="O15:O17" si="5">E37*E13/100</f>
         <v>76.137</v>
       </c>
-      <c r="P15" s="58">
+      <c r="P15" s="50">
         <v>39.4</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="48"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -1710,7 +1726,7 @@
         <f t="shared" si="5"/>
         <v>87.875</v>
       </c>
-      <c r="P16" s="58">
+      <c r="P16" s="50">
         <v>65</v>
       </c>
     </row>
@@ -1743,22 +1759,22 @@
         <f t="shared" si="5"/>
         <v>38.76</v>
       </c>
-      <c r="P17" s="59">
+      <c r="P17" s="51">
         <v>38.5</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="42" t="s">
+      <c r="C18" s="64"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="43"/>
-      <c r="G18" s="44"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="65"/>
       <c r="H18" s="32" t="s">
         <v>8</v>
       </c>
@@ -1936,16 +1952,16 @@
     </row>
     <row r="26" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="43"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="42" t="s">
+      <c r="C26" s="64"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="F26" s="43"/>
-      <c r="G26" s="44"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="65"/>
       <c r="H26" s="32" t="s">
         <v>8</v>
       </c>
@@ -2123,16 +2139,16 @@
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
-      <c r="B34" s="42" t="s">
+      <c r="B34" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="43"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="42" t="s">
+      <c r="C34" s="64"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="F34" s="43"/>
-      <c r="G34" s="44"/>
+      <c r="F34" s="64"/>
+      <c r="G34" s="65"/>
       <c r="H34" s="32" t="s">
         <v>8</v>
       </c>
@@ -2293,7 +2309,7 @@
         <v>8.8127999999999993</v>
       </c>
       <c r="J39" s="31" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
@@ -2322,16 +2338,16 @@
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="14"/>
-      <c r="B42" s="45" t="s">
+      <c r="B42" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="46"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="45" t="s">
+      <c r="C42" s="67"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="F42" s="46"/>
-      <c r="G42" s="47"/>
+      <c r="F42" s="67"/>
+      <c r="G42" s="68"/>
       <c r="H42" s="32" t="s">
         <v>8</v>
       </c>
@@ -2527,16 +2543,16 @@
     </row>
     <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
-      <c r="B51" s="42" t="s">
+      <c r="B51" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="43"/>
-      <c r="D51" s="44"/>
-      <c r="E51" s="42" t="s">
+      <c r="C51" s="64"/>
+      <c r="D51" s="65"/>
+      <c r="E51" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="F51" s="43"/>
-      <c r="G51" s="44"/>
+      <c r="F51" s="64"/>
+      <c r="G51" s="65"/>
       <c r="H51" s="32" t="s">
         <v>8</v>
       </c>
@@ -2698,43 +2714,43 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="55"/>
+      <c r="A57" s="47"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
-      <c r="H57" s="56"/>
-      <c r="I57" s="56"/>
+      <c r="H57" s="48"/>
+      <c r="I57" s="48"/>
     </row>
     <row r="58" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="B58" s="49"/>
-      <c r="C58" s="49"/>
-      <c r="D58" s="49"/>
-      <c r="E58" s="49"/>
-      <c r="F58" s="49"/>
-      <c r="G58" s="49"/>
-      <c r="H58" s="56"/>
-      <c r="I58" s="56"/>
+      <c r="A58" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="B58" s="41"/>
+      <c r="C58" s="41"/>
+      <c r="D58" s="41"/>
+      <c r="E58" s="41"/>
+      <c r="F58" s="41"/>
+      <c r="G58" s="41"/>
+      <c r="H58" s="48"/>
+      <c r="I58" s="48"/>
     </row>
     <row r="59" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="14"/>
-      <c r="B59" s="42" t="s">
+      <c r="B59" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="43"/>
-      <c r="D59" s="44"/>
-      <c r="E59" s="42" t="s">
+      <c r="C59" s="64"/>
+      <c r="D59" s="65"/>
+      <c r="E59" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="F59" s="43"/>
-      <c r="G59" s="44"/>
-      <c r="H59" s="56"/>
-      <c r="I59" s="56"/>
+      <c r="F59" s="64"/>
+      <c r="G59" s="65"/>
+      <c r="H59" s="48"/>
+      <c r="I59" s="48"/>
     </row>
     <row r="60" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
@@ -2758,8 +2774,8 @@
       <c r="G60" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H60" s="56"/>
-      <c r="I60" s="56"/>
+      <c r="H60" s="48"/>
+      <c r="I60" s="48"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="18">
@@ -2783,8 +2799,8 @@
       <c r="G61" s="9">
         <v>5</v>
       </c>
-      <c r="H61" s="56"/>
-      <c r="I61" s="56"/>
+      <c r="H61" s="48"/>
+      <c r="I61" s="48"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="18">
@@ -2808,8 +2824,8 @@
       <c r="G62" s="9">
         <v>5</v>
       </c>
-      <c r="H62" s="56"/>
-      <c r="I62" s="56"/>
+      <c r="H62" s="48"/>
+      <c r="I62" s="48"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="18">
@@ -2833,8 +2849,8 @@
       <c r="G63" s="9">
         <v>5</v>
       </c>
-      <c r="H63" s="56"/>
-      <c r="I63" s="56"/>
+      <c r="H63" s="48"/>
+      <c r="I63" s="48"/>
     </row>
     <row r="64" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="19">
@@ -2858,8 +2874,8 @@
       <c r="G64" s="13">
         <v>6</v>
       </c>
-      <c r="H64" s="56"/>
-      <c r="I64" s="56"/>
+      <c r="H64" s="48"/>
+      <c r="I64" s="48"/>
     </row>
     <row r="66" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="30" t="s">
@@ -2878,16 +2894,16 @@
     </row>
     <row r="67" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="29"/>
-      <c r="B67" s="42" t="s">
+      <c r="B67" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C67" s="43"/>
-      <c r="D67" s="44"/>
-      <c r="E67" s="42" t="s">
+      <c r="C67" s="64"/>
+      <c r="D67" s="65"/>
+      <c r="E67" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="F67" s="43"/>
-      <c r="G67" s="44"/>
+      <c r="F67" s="64"/>
+      <c r="G67" s="65"/>
       <c r="H67" s="32" t="s">
         <v>8</v>
       </c>
@@ -3163,7 +3179,7 @@
         <v>29</v>
       </c>
       <c r="E85" s="31" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F85" s="31" t="s">
         <v>37</v>
@@ -3227,7 +3243,7 @@
         <v>29</v>
       </c>
       <c r="E89" s="31" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F89" s="31" t="s">
         <v>37</v>
@@ -3282,10 +3298,10 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="31" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E93" s="31" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -3385,7 +3401,7 @@
     </row>
     <row r="103" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A103" s="31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="104" spans="1:27" x14ac:dyDescent="0.2">
@@ -3423,69 +3439,69 @@
       </c>
     </row>
     <row r="109" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="60" t="s">
-        <v>79</v>
-      </c>
-      <c r="B109" s="61"/>
-      <c r="C109" s="61"/>
-      <c r="D109" s="61"/>
-      <c r="E109" s="61"/>
-      <c r="F109" s="61"/>
-      <c r="G109" s="61"/>
-      <c r="H109" s="61"/>
-      <c r="I109" s="61"/>
-      <c r="J109" s="61"/>
-      <c r="K109" s="61"/>
-      <c r="L109" s="61"/>
-      <c r="M109" s="61"/>
-      <c r="N109" s="61"/>
-      <c r="O109" s="61"/>
-      <c r="P109" s="61"/>
-      <c r="Q109" s="61"/>
-      <c r="R109" s="61"/>
-      <c r="S109" s="61"/>
-      <c r="T109" s="61"/>
-      <c r="U109" s="61"/>
-      <c r="V109" s="61"/>
-      <c r="W109" s="61"/>
-      <c r="X109" s="61"/>
-      <c r="Y109" s="61"/>
+      <c r="A109" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="B109" s="53"/>
+      <c r="C109" s="53"/>
+      <c r="D109" s="53"/>
+      <c r="E109" s="53"/>
+      <c r="F109" s="53"/>
+      <c r="G109" s="53"/>
+      <c r="H109" s="53"/>
+      <c r="I109" s="53"/>
+      <c r="J109" s="53"/>
+      <c r="K109" s="53"/>
+      <c r="L109" s="53"/>
+      <c r="M109" s="53"/>
+      <c r="N109" s="53"/>
+      <c r="O109" s="53"/>
+      <c r="P109" s="53"/>
+      <c r="Q109" s="53"/>
+      <c r="R109" s="53"/>
+      <c r="S109" s="53"/>
+      <c r="T109" s="53"/>
+      <c r="U109" s="53"/>
+      <c r="V109" s="53"/>
+      <c r="W109" s="53"/>
+      <c r="X109" s="53"/>
+      <c r="Y109" s="53"/>
     </row>
     <row r="110" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="62"/>
-      <c r="B110" s="63" t="s">
+      <c r="A110" s="54"/>
+      <c r="B110" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C110" s="64"/>
-      <c r="D110" s="64"/>
-      <c r="E110" s="64"/>
-      <c r="F110" s="64"/>
-      <c r="G110" s="64"/>
-      <c r="H110" s="64"/>
-      <c r="I110" s="64"/>
-      <c r="J110" s="64"/>
-      <c r="K110" s="64"/>
-      <c r="L110" s="64"/>
-      <c r="M110" s="65"/>
-      <c r="N110" s="68" t="s">
-        <v>81</v>
-      </c>
-      <c r="O110" s="63" t="s">
+      <c r="C110" s="61"/>
+      <c r="D110" s="61"/>
+      <c r="E110" s="61"/>
+      <c r="F110" s="61"/>
+      <c r="G110" s="61"/>
+      <c r="H110" s="61"/>
+      <c r="I110" s="61"/>
+      <c r="J110" s="61"/>
+      <c r="K110" s="61"/>
+      <c r="L110" s="61"/>
+      <c r="M110" s="62"/>
+      <c r="N110" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="O110" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="P110" s="64"/>
-      <c r="Q110" s="64"/>
-      <c r="R110" s="64"/>
-      <c r="S110" s="64"/>
-      <c r="T110" s="64"/>
-      <c r="U110" s="64"/>
-      <c r="V110" s="64"/>
-      <c r="W110" s="64"/>
-      <c r="X110" s="64"/>
-      <c r="Y110" s="64"/>
-      <c r="Z110" s="64"/>
-      <c r="AA110" s="69" t="s">
-        <v>83</v>
+      <c r="P110" s="61"/>
+      <c r="Q110" s="61"/>
+      <c r="R110" s="61"/>
+      <c r="S110" s="61"/>
+      <c r="T110" s="61"/>
+      <c r="U110" s="61"/>
+      <c r="V110" s="61"/>
+      <c r="W110" s="61"/>
+      <c r="X110" s="61"/>
+      <c r="Y110" s="61"/>
+      <c r="Z110" s="61"/>
+      <c r="AA110" s="58" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="111" spans="1:27" x14ac:dyDescent="0.2">
@@ -3763,74 +3779,74 @@
       </c>
     </row>
     <row r="115" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="AA115" s="56"/>
+      <c r="AA115" s="48"/>
     </row>
     <row r="116" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="60" t="s">
-        <v>80</v>
-      </c>
-      <c r="B116" s="60"/>
-      <c r="C116" s="60"/>
-      <c r="D116" s="60"/>
-      <c r="E116" s="60"/>
-      <c r="F116" s="60"/>
-      <c r="G116" s="60"/>
-      <c r="H116" s="60"/>
-      <c r="I116" s="60"/>
-      <c r="J116" s="60"/>
-      <c r="K116" s="60"/>
-      <c r="L116" s="60"/>
-      <c r="M116" s="60"/>
-      <c r="N116" s="60"/>
-      <c r="O116" s="60"/>
-      <c r="P116" s="60"/>
-      <c r="Q116" s="60"/>
-      <c r="R116" s="60"/>
-      <c r="S116" s="60"/>
-      <c r="T116" s="60"/>
-      <c r="U116" s="60"/>
-      <c r="V116" s="60"/>
-      <c r="W116" s="60"/>
-      <c r="X116" s="60"/>
-      <c r="Y116" s="60"/>
-      <c r="Z116" s="60"/>
-      <c r="AA116" s="56"/>
+      <c r="A116" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="B116" s="52"/>
+      <c r="C116" s="52"/>
+      <c r="D116" s="52"/>
+      <c r="E116" s="52"/>
+      <c r="F116" s="52"/>
+      <c r="G116" s="52"/>
+      <c r="H116" s="52"/>
+      <c r="I116" s="52"/>
+      <c r="J116" s="52"/>
+      <c r="K116" s="52"/>
+      <c r="L116" s="52"/>
+      <c r="M116" s="52"/>
+      <c r="N116" s="52"/>
+      <c r="O116" s="52"/>
+      <c r="P116" s="52"/>
+      <c r="Q116" s="52"/>
+      <c r="R116" s="52"/>
+      <c r="S116" s="52"/>
+      <c r="T116" s="52"/>
+      <c r="U116" s="52"/>
+      <c r="V116" s="52"/>
+      <c r="W116" s="52"/>
+      <c r="X116" s="52"/>
+      <c r="Y116" s="52"/>
+      <c r="Z116" s="52"/>
+      <c r="AA116" s="48"/>
     </row>
     <row r="117" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="66"/>
-      <c r="B117" s="63" t="s">
+      <c r="A117" s="55"/>
+      <c r="B117" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C117" s="64"/>
-      <c r="D117" s="64"/>
-      <c r="E117" s="64"/>
-      <c r="F117" s="64"/>
-      <c r="G117" s="64"/>
-      <c r="H117" s="64"/>
-      <c r="I117" s="64"/>
-      <c r="J117" s="64"/>
-      <c r="K117" s="64"/>
-      <c r="L117" s="64"/>
-      <c r="M117" s="65"/>
-      <c r="N117" s="68" t="s">
-        <v>82</v>
-      </c>
-      <c r="O117" s="63" t="s">
+      <c r="C117" s="61"/>
+      <c r="D117" s="61"/>
+      <c r="E117" s="61"/>
+      <c r="F117" s="61"/>
+      <c r="G117" s="61"/>
+      <c r="H117" s="61"/>
+      <c r="I117" s="61"/>
+      <c r="J117" s="61"/>
+      <c r="K117" s="61"/>
+      <c r="L117" s="61"/>
+      <c r="M117" s="62"/>
+      <c r="N117" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="O117" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="P117" s="64"/>
-      <c r="Q117" s="64"/>
-      <c r="R117" s="64"/>
-      <c r="S117" s="64"/>
-      <c r="T117" s="64"/>
-      <c r="U117" s="64"/>
-      <c r="V117" s="64"/>
-      <c r="W117" s="64"/>
-      <c r="X117" s="64"/>
-      <c r="Y117" s="64"/>
-      <c r="Z117" s="64"/>
-      <c r="AA117" s="70" t="s">
-        <v>84</v>
+      <c r="P117" s="61"/>
+      <c r="Q117" s="61"/>
+      <c r="R117" s="61"/>
+      <c r="S117" s="61"/>
+      <c r="T117" s="61"/>
+      <c r="U117" s="61"/>
+      <c r="V117" s="61"/>
+      <c r="W117" s="61"/>
+      <c r="X117" s="61"/>
+      <c r="Y117" s="61"/>
+      <c r="Z117" s="61"/>
+      <c r="AA117" s="59" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="118" spans="1:27" x14ac:dyDescent="0.2">
@@ -4035,7 +4051,7 @@
       <c r="D121" s="12">
         <v>5120.54</v>
       </c>
-      <c r="E121" s="67"/>
+      <c r="E121" s="56"/>
       <c r="F121" s="12">
         <v>5064.42</v>
       </c>
@@ -4094,8 +4110,8 @@
       <c r="X121" s="12">
         <v>2458.42</v>
       </c>
-      <c r="Y121" s="67"/>
-      <c r="Z121" s="67"/>
+      <c r="Y121" s="56"/>
+      <c r="Z121" s="56"/>
       <c r="AA121" s="34">
         <f>AVERAGE(O121:X121)</f>
         <v>4239.0460000000003</v>
@@ -4103,18 +4119,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B110:M110"/>
-    <mergeCell ref="O110:Z110"/>
-    <mergeCell ref="B117:M117"/>
-    <mergeCell ref="O117:Z117"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="L5:P5"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="L4:P4"/>
     <mergeCell ref="B59:D59"/>
     <mergeCell ref="E59:G59"/>
     <mergeCell ref="B2:D2"/>
@@ -4125,11 +4134,18 @@
     <mergeCell ref="E26:G26"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="E10:G10"/>
-    <mergeCell ref="L1:P1"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="L5:P5"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="L4:P4"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="B110:M110"/>
+    <mergeCell ref="O110:Z110"/>
+    <mergeCell ref="B117:M117"/>
+    <mergeCell ref="O117:Z117"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="E67:G67"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4526,7 +4542,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4534,9 +4550,9 @@
     <col min="1" max="16384" width="9" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B1" s="31">
         <v>24</v>
@@ -4547,38 +4563,47 @@
       <c r="D1" s="31">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="31">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="56">
-        <v>633.40563991323199</v>
-      </c>
-      <c r="C2" s="56">
-        <v>777.10437710437714</v>
-      </c>
-      <c r="D2" s="56">
-        <v>769.50819672131138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="B2" s="31">
+        <v>341.40563991323205</v>
+      </c>
+      <c r="C2" s="31">
+        <v>315.50437710437711</v>
+      </c>
+      <c r="D2" s="31">
+        <v>300.10819672131146</v>
+      </c>
+      <c r="E2" s="31">
+        <v>190.27968337730874</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="B3" s="31">
-        <v>682.09876543209884</v>
+        <v>240.09876543209882</v>
       </c>
       <c r="C3" s="31">
-        <v>830.87248322147639</v>
+        <v>211.8724832214765</v>
       </c>
       <c r="D3" s="31">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="E3" s="31">
+        <v>154.81481481481481</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="B5" s="31">
         <v>24</v>
@@ -4589,24 +4614,30 @@
       <c r="D5" s="31">
         <v>96</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="31">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="56">
+        <v>90</v>
+      </c>
+      <c r="B6" s="48">
         <v>60.998800000000003</v>
       </c>
-      <c r="C6" s="56">
+      <c r="C6" s="48">
         <v>77.13336000000001</v>
       </c>
-      <c r="D6" s="56">
+      <c r="D6" s="48">
         <v>116.50507999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="31">
+        <v>216.22880000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="B7" s="31">
         <v>108.29</v>
@@ -4617,10 +4648,13 @@
       <c r="D7" s="31">
         <v>247.87779999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="31">
+        <v>107.73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="B9" s="31">
         <v>24</v>
@@ -4631,24 +4665,30 @@
       <c r="D9" s="31">
         <v>96</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="31">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="56">
+        <v>8</v>
+      </c>
+      <c r="B10" s="48">
         <v>21.520399999999999</v>
       </c>
-      <c r="C10" s="56">
+      <c r="C10" s="48">
         <v>60.931199999999997</v>
       </c>
-      <c r="D10" s="56">
+      <c r="D10" s="48">
         <v>68.062999999999988</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="31">
+        <v>99.531999999999982</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="B11" s="31">
         <v>27.846</v>
@@ -4659,10 +4699,13 @@
       <c r="D11" s="31">
         <v>87.875</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="31">
+        <v>38.76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="B13" s="31">
         <v>24</v>
@@ -4673,24 +4716,30 @@
       <c r="D13" s="31">
         <v>96</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="31">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="56">
+      <c r="B14" s="48">
         <v>45.1</v>
       </c>
-      <c r="C14" s="56">
+      <c r="C14" s="48">
         <v>56.2</v>
       </c>
-      <c r="D14" s="56">
+      <c r="D14" s="48">
         <v>61</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="31">
+        <v>70.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="B15" s="31">
         <v>44.1</v>
@@ -4700,6 +4749,9 @@
       </c>
       <c r="D15" s="31">
         <v>65</v>
+      </c>
+      <c r="E15" s="31">
+        <v>38.5</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -4764,7 +4816,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B19" s="31">
         <v>0</v>
@@ -4793,7 +4845,7 @@
     </row>
     <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="31" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="B21" s="31">
         <v>24</v>
@@ -4818,19 +4870,19 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="31" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="B22" s="31">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C22" s="31">
-        <v>0.08</v>
+        <v>10</v>
       </c>
       <c r="D22" s="31">
-        <v>0.1</v>
+        <v>20</v>
       </c>
       <c r="E22" s="31">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="F22" s="31">
         <v>28.120002343333312</v>
@@ -4841,19 +4893,19 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="31" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="B23" s="31">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C23" s="31">
-        <v>0.08</v>
+        <v>10</v>
       </c>
       <c r="D23" s="31">
-        <v>0.1</v>
+        <v>20</v>
       </c>
       <c r="E23" s="31">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="F23" s="31">
         <v>25.308000000000007</v>
@@ -4864,7 +4916,7 @@
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="31" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="B25" s="31">
         <v>24</v>
@@ -4889,19 +4941,19 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="31" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B26" s="31">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C26" s="31">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="D26" s="31">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="E26" s="31">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="F26" s="31">
         <v>131.22666666666669</v>
@@ -4912,19 +4964,19 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="31" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="B27" s="31">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C27" s="31">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="D27" s="31">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="E27" s="31">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="F27" s="31">
         <v>110.23039999999999</v>
@@ -4935,7 +4987,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="31" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B29" s="31">
         <v>24</v>
@@ -4969,7 +5021,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B31" s="31">
         <v>6.1480000000000006</v>
@@ -4986,7 +5038,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="31" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B33" s="31">
         <v>24</v>
@@ -5020,7 +5072,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B35" s="31">
         <v>17.032</v>
@@ -5038,5 +5090,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>